<commit_message>
added a third application file for January 2023
</commit_message>
<xml_diff>
--- a/my classes schedule.xlsx
+++ b/my classes schedule.xlsx
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="203">
   <si>
     <t>Saturday</t>
   </si>
@@ -594,9 +595,6 @@
     <t>1401/07/14</t>
   </si>
   <si>
-    <t>جلسه توجیهی موسسه دهخدا ساعت 15</t>
-  </si>
-  <si>
     <t>رضا ساعت 4</t>
   </si>
   <si>
@@ -604,6 +602,39 @@
   </si>
   <si>
     <t>1401/07/24</t>
+  </si>
+  <si>
+    <t>کلاس آنلاین با صبا خانم ساعت 10</t>
+  </si>
+  <si>
+    <t>username: melli code</t>
+  </si>
+  <si>
+    <t>password: melli code</t>
+  </si>
+  <si>
+    <t>I should be present in the application 15 minutes before start of the class</t>
+  </si>
+  <si>
+    <t>private classes: 10 sessions</t>
+  </si>
+  <si>
+    <t>public classes: 14 sessions - last session = final exam</t>
+  </si>
+  <si>
+    <t>Dehkhoda Institute's requirements:</t>
+  </si>
+  <si>
+    <t>no one should be absent for more than 2 to 3 sessions, otherwise I should report</t>
+  </si>
+  <si>
+    <t>inform the institute one month in advance for any resignation of cooperation contract</t>
+  </si>
+  <si>
+    <t>مینا عابدی شاگرد اصفهان</t>
+  </si>
+  <si>
+    <t>1401/07/28</t>
   </si>
 </sst>
 </file>
@@ -613,7 +644,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -630,6 +661,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -759,7 +798,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -830,6 +869,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1110,10 +1153,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q49"/>
+  <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J52" sqref="J52"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1593,7 +1636,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B26" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C26" s="27"/>
       <c r="D26" s="27"/>
@@ -1808,7 +1851,7 @@
         <v>178</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">
@@ -2085,10 +2128,18 @@
         <v>187</v>
       </c>
       <c r="N49" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2101,8 +2152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2209,9 +2260,7 @@
       </c>
       <c r="Q2" s="13"/>
       <c r="R2" s="15"/>
-      <c r="S2" s="28" t="s">
-        <v>189</v>
-      </c>
+      <c r="S2" s="28"/>
       <c r="T2" s="13"/>
       <c r="U2" s="13"/>
     </row>
@@ -2338,6 +2387,9 @@
       </c>
       <c r="Q7" s="17"/>
       <c r="R7" s="19"/>
+      <c r="S7" s="30" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
@@ -2361,10 +2413,69 @@
       <c r="Q8" s="21"/>
       <c r="R8" s="23"/>
       <c r="S8" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="T8" s="23"/>
       <c r="U8" s="23"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="72.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>200</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>